<commit_message>
updated points considered 'done'.
</commit_message>
<xml_diff>
--- a/DOCS/CCED Metric.xlsx
+++ b/DOCS/CCED Metric.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matto\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Connor\Desktop\Lewis\Year 4 - Semester 2\Software Systems Capstone\Software-Systems-Capstone\UltimateSeatSelector\DOCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD7D6318-9067-4AAC-9CCA-FBF1E9281CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694B9A94-44F7-4FED-A4CF-C9B2BDB6FB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint5" sheetId="1" r:id="rId1"/>
@@ -515,19 +515,19 @@
   <dimension ref="A1:I1004"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.3125" customWidth="1"/>
-    <col min="2" max="5" width="5.3125" customWidth="1"/>
+    <col min="1" max="1" width="17.296875" customWidth="1"/>
+    <col min="2" max="5" width="5.296875" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="9" width="6" customWidth="1"/>
     <col min="10" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25">
+    <row r="1" spans="1:9" ht="23.4">
       <c r="A1" s="13" t="s">
         <v>33</v>
       </c>
@@ -655,7 +655,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="9">
@@ -664,11 +664,11 @@
       </c>
       <c r="H10" s="10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="I10" s="10">
         <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1">
@@ -685,7 +685,7 @@
         <v>12</v>
       </c>
       <c r="E11" s="7">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9">
@@ -694,11 +694,11 @@
       </c>
       <c r="H11" s="10">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="I11" s="10">
         <f t="shared" si="1"/>
-        <v>0.8571428571428571</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1">
@@ -730,7 +730,7 @@
       </c>
       <c r="E13" s="7">
         <f>SUM(E9:E11)</f>
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="9">
@@ -739,11 +739,11 @@
       </c>
       <c r="H13" s="10">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.83783783783783783</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="1"/>
-        <v>0.88095238095238093</v>
+        <v>0.73809523809523814</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1">
@@ -6755,16 +6755,16 @@
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.3125" customWidth="1"/>
-    <col min="2" max="5" width="5.3125" customWidth="1"/>
+    <col min="1" max="1" width="17.296875" customWidth="1"/>
+    <col min="2" max="5" width="5.296875" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="9" width="6" customWidth="1"/>
     <col min="10" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25">
+    <row r="1" spans="1:9" ht="23.4">
       <c r="A1" s="13" t="str">
         <f>Sprint5!A1</f>
         <v>Capacity, Committed, Effort, and Delivered Metric</v>
@@ -13106,16 +13106,16 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.3125" customWidth="1"/>
-    <col min="2" max="5" width="5.3125" customWidth="1"/>
+    <col min="1" max="1" width="17.296875" customWidth="1"/>
+    <col min="2" max="5" width="5.296875" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="9" width="6" customWidth="1"/>
     <col min="10" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25">
+    <row r="1" spans="1:9" ht="23.4">
       <c r="A1" s="13" t="str">
         <f>Sprint5!A1</f>
         <v>Capacity, Committed, Effort, and Delivered Metric</v>
@@ -19457,16 +19457,16 @@
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="17.3125" customWidth="1"/>
-    <col min="2" max="5" width="5.3125" customWidth="1"/>
+    <col min="1" max="1" width="17.296875" customWidth="1"/>
+    <col min="2" max="5" width="5.296875" customWidth="1"/>
     <col min="6" max="6" width="3" customWidth="1"/>
     <col min="7" max="9" width="6" customWidth="1"/>
     <col min="10" max="26" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="23.25">
+    <row r="1" spans="1:9" ht="23.4">
       <c r="A1" s="13" t="str">
         <f>Sprint5!A1</f>
         <v>Capacity, Committed, Effort, and Delivered Metric</v>

</xml_diff>